<commit_message>
output graph push to remote
</commit_message>
<xml_diff>
--- a/outputWB.xlsx
+++ b/outputWB.xlsx
@@ -462,7 +462,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0</v>
+        <v>64</v>
       </c>
       <c r="C2" t="n">
         <v>0</v>
@@ -507,19 +507,19 @@
         <v>63</v>
       </c>
       <c r="Q2" t="n">
-        <v>14</v>
+        <v>53</v>
       </c>
       <c r="R2" t="n">
-        <v>0</v>
+        <v>147</v>
       </c>
       <c r="S2" t="n">
-        <v>0</v>
+        <v>118</v>
       </c>
       <c r="T2" t="n">
-        <v>0</v>
+        <v>132</v>
       </c>
       <c r="U2" t="n">
-        <v>0</v>
+        <v>52</v>
       </c>
     </row>
     <row r="3">
@@ -529,7 +529,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0</v>
+        <v>76</v>
       </c>
       <c r="C3" t="n">
         <v>0</v>
@@ -574,19 +574,19 @@
         <v>92</v>
       </c>
       <c r="Q3" t="n">
-        <v>28</v>
+        <v>102</v>
       </c>
       <c r="R3" t="n">
-        <v>0</v>
+        <v>235</v>
       </c>
       <c r="S3" t="n">
-        <v>0</v>
+        <v>177</v>
       </c>
       <c r="T3" t="n">
-        <v>0</v>
+        <v>189</v>
       </c>
       <c r="U3" t="n">
-        <v>0</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>

</xml_diff>